<commit_message>
Added temp data to excel sheet
</commit_message>
<xml_diff>
--- a/Membership Proposal Details.xlsx
+++ b/Membership Proposal Details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtxhq-my.sharepoint.com/personal/john_lee_venturex_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabekrishnadasan/Desktop/VentureX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{1440901B-9D65-5D4C-8BA9-CFF86D9750C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CF1902F-6E42-664E-AF96-8B900C7DCAC4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32384FA2-E1F7-F140-A512-CFD8D184174A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17920" yWindow="500" windowWidth="26880" windowHeight="20460" activeTab="1" xr2:uid="{804F3DE6-0492-F647-A008-134247438643}"/>
+    <workbookView xWindow="-38400" yWindow="-1780" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{804F3DE6-0492-F647-A008-134247438643}"/>
   </bookViews>
   <sheets>
     <sheet name="Client Info" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Full Name</t>
   </si>
@@ -327,13 +327,25 @@
   </si>
   <si>
     <t>XXX</t>
+  </si>
+  <si>
+    <t>Gabriel Krishnadasan</t>
+  </si>
+  <si>
+    <t>Temp Name</t>
+  </si>
+  <si>
+    <t>email@gmail.com</t>
+  </si>
+  <si>
+    <t>(206)128-5555</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -354,6 +366,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -372,10 +392,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -383,8 +404,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,14 +423,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -445,7 +464,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -551,7 +570,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -693,7 +712,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -701,38 +720,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0B81AC-30C4-8A41-8B47-57C3ECEAE88B}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{C23E1B77-0FE6-954D-A52B-2ED691216A86}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -742,7 +777,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Replaced text on slide 6
</commit_message>
<xml_diff>
--- a/Membership Proposal Details.xlsx
+++ b/Membership Proposal Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabekrishnadasan/Desktop/VentureX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB15D9A-BC44-AD4F-8808-D36DE438E1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4811A8-DE0B-DA43-8D7C-B34F91593509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{804F3DE6-0492-F647-A008-134247438643}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{804F3DE6-0492-F647-A008-134247438643}"/>
   </bookViews>
   <sheets>
     <sheet name="Client Info" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Full Name</t>
   </si>
@@ -323,9 +323,6 @@
     <t>Additional Fees</t>
   </si>
   <si>
-    <t>General Comment Section</t>
-  </si>
-  <si>
     <t>XXX</t>
   </si>
   <si>
@@ -345,6 +342,9 @@
   </si>
   <si>
     <t>Microsoft</t>
+  </si>
+  <si>
+    <t>General Comment Section Hello</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0B81AC-30C4-8A41-8B47-57C3ECEAE88B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -768,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8FF8D7-401D-D140-9586-5CDB09824088}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,13 +812,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -826,7 +829,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -858,7 +861,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -866,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -874,7 +877,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Edited to present to John
</commit_message>
<xml_diff>
--- a/Membership Proposal Details.xlsx
+++ b/Membership Proposal Details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabekrishnadasan/Desktop/VentureX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4849200E-52BA-534F-8BA6-11A4BEC6EB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6757CFE6-121D-8C4B-A5B3-27828AE9FA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{804F3DE6-0492-F647-A008-134247438643}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18060" windowHeight="16400" activeTab="1" xr2:uid="{804F3DE6-0492-F647-A008-134247438643}"/>
   </bookViews>
   <sheets>
     <sheet name="Client Info" sheetId="1" r:id="rId1"/>
@@ -281,9 +281,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Term</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -341,7 +338,10 @@
     <t>Microsoft</t>
   </si>
   <si>
-    <t>General Comment Section Hello</t>
+    <t>Term (Months)</t>
+  </si>
+  <si>
+    <t>General Comment Section</t>
   </si>
 </sst>
 </file>
@@ -428,9 +428,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -468,7 +468,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -574,7 +574,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -716,7 +716,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -727,7 +727,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -749,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -757,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -765,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -781,7 +781,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +798,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -809,16 +809,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -831,7 +831,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
         <v>45327</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
         <v>45509</v>
@@ -855,41 +855,41 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>